<commit_message>
updated uml and Compare the cost effectiveness of the two routing methods
</commit_message>
<xml_diff>
--- a/Sprints/Sprint 3 Backlog and Burndown Chart.xlsx
+++ b/Sprints/Sprint 3 Backlog and Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Classes/CSCI 234 - Software Engineering/Projects/Project03/Sprints/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AbdullahAlramyan/Desktop/CSCI/IntroSoftwareEngineering/Project03/Sprints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789C984-A8BA-FD47-B147-2047B1C916B7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76A9BEB-9919-884B-853C-CB3DDAD1BADB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>User Story #1</t>
   </si>
@@ -171,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Update Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">complete </t>
   </si>
 </sst>
 </file>
@@ -394,7 +398,7 @@
             <c:strRef>
               <c:f>'Agile Sprint Backlog'!$G$2:$Q$2</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>DAY 1</c:v>
                 </c:pt>
@@ -423,9 +427,6 @@
                   <c:v>DAY 9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>DAY 10</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>SPRINT REVIEW</c:v>
                 </c:pt>
               </c:strCache>
@@ -436,38 +437,35 @@
               <c:f>'Agile Sprint Backlog'!$G$30:$Q$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -948,9 +946,9 @@
   </sheetPr>
   <dimension ref="B1:AG126"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -961,7 +959,8 @@
     <col min="4" max="4" width="35.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="3" customWidth="1"/>
-    <col min="7" max="16" width="10.83203125" style="3"/>
+    <col min="7" max="15" width="10.83203125" style="3"/>
+    <col min="16" max="16" width="0" style="3" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" style="3" customWidth="1"/>
     <col min="18" max="18" width="1.83203125" style="3" customWidth="1"/>
     <col min="19" max="25" width="10.83203125" style="3"/>
@@ -1875,22 +1874,48 @@
       <c r="B18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>7</v>
+      </c>
       <c r="D18" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="8">
+        <v>5</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
+        <v>2</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="N18" s="8">
+        <v>8</v>
+      </c>
+      <c r="O18" s="8">
+        <v>2</v>
+      </c>
+      <c r="P18" s="8">
+        <v>1</v>
+      </c>
       <c r="Q18" s="8"/>
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
@@ -1913,22 +1938,48 @@
       <c r="B19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
       <c r="D19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="8">
+        <v>13</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="8">
+        <v>1</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1</v>
+      </c>
+      <c r="K19" s="8">
+        <v>0</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0</v>
+      </c>
+      <c r="N19" s="8">
+        <v>0</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0</v>
+      </c>
+      <c r="P19" s="8">
+        <v>0</v>
+      </c>
       <c r="Q19" s="8"/>
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
@@ -2316,47 +2367,47 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5">
         <f>SUM(F3:F29)</f>
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="G30" s="5">
         <f>SUM(G4:G29)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ref="H30:Q30" si="0">SUM(H3:H29)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>31.5</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L30" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M30" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O30" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q30" s="5">
         <f t="shared" si="0"/>

</xml_diff>